<commit_message>
1. add 'setPath' method 2.add 'loadingNode' option
</commit_message>
<xml_diff>
--- a/api/api.xlsx
+++ b/api/api.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="核心类-Svideo" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="186">
   <si>
     <t>Svideo</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -163,14 +163,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>添加播放资源</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>移除当前的播放资源</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>play( )</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -747,6 +739,30 @@
   </si>
   <si>
     <t>资源类型 mp4: 常规video支持的资源类型总称  m3u8: HLS直播流格式</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>添加播放资源（已放弃维护该方法，请使用 setPath(String)）</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>移除当前的播放资源（已抛弃的方法，不建议使用）</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>setPath(String:path)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>设置视频资源，例如 video.setPath('XXXXX.mp4')</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>loadingNode</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>自定义加载节点，可以为html节点或者字符串</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1209,10 +1225,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D67"/>
+  <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -1235,7 +1251,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -1342,558 +1358,578 @@
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="1" t="s">
-        <v>20</v>
+        <v>184</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>21</v>
+        <v>185</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="8"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
-      <c r="B18" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>31</v>
-      </c>
+      <c r="B18" s="6"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="8"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
+      <c r="B19" s="4" t="s">
+        <v>29</v>
+      </c>
       <c r="C19" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="1" t="s">
-        <v>34</v>
+        <v>182</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>35</v>
+        <v>183</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>39</v>
+        <v>180</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>41</v>
+        <v>181</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="1" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="1" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
       <c r="C43" s="1" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
       <c r="B44" s="4"/>
       <c r="C44" s="1" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
       <c r="B45" s="4"/>
       <c r="C45" s="1" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
       <c r="B46" s="4"/>
       <c r="C46" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
       <c r="B47" s="4"/>
       <c r="C47" s="1" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="4"/>
       <c r="B48" s="4"/>
       <c r="C48" s="1" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="4"/>
-      <c r="B49" s="6"/>
-      <c r="C49" s="7"/>
-      <c r="D49" s="8"/>
+      <c r="B49" s="4"/>
+      <c r="C49" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="4"/>
-      <c r="B50" s="4" t="s">
-        <v>92</v>
-      </c>
+      <c r="B50" s="4"/>
       <c r="C50" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>3</v>
+        <v>89</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="4"/>
-      <c r="B51" s="4"/>
-      <c r="C51" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>95</v>
-      </c>
+      <c r="B51" s="6"/>
+      <c r="C51" s="7"/>
+      <c r="D51" s="8"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="4"/>
-      <c r="B52" s="4"/>
+      <c r="B52" s="4" t="s">
+        <v>90</v>
+      </c>
       <c r="C52" s="1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>97</v>
+        <v>3</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="4"/>
       <c r="B53" s="4"/>
       <c r="C53" s="1" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="4"/>
       <c r="B54" s="4"/>
       <c r="C54" s="1" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="4"/>
       <c r="B55" s="4"/>
       <c r="C55" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="4"/>
       <c r="B56" s="4"/>
       <c r="C56" s="1" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="4"/>
       <c r="B57" s="4"/>
       <c r="C57" s="1" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="4"/>
       <c r="B58" s="4"/>
       <c r="C58" s="1" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="4"/>
       <c r="B59" s="4"/>
-      <c r="C59" s="2" t="s">
-        <v>110</v>
+      <c r="C59" s="1" t="s">
+        <v>104</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="4"/>
       <c r="B60" s="4"/>
       <c r="C60" s="1" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="4"/>
       <c r="B61" s="4"/>
-      <c r="C61" s="1" t="s">
-        <v>114</v>
+      <c r="C61" s="2" t="s">
+        <v>108</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="4"/>
       <c r="B62" s="4"/>
       <c r="C62" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="4"/>
       <c r="B63" s="4"/>
       <c r="C63" s="1" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="4"/>
       <c r="B64" s="4"/>
       <c r="C64" s="1" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="4"/>
       <c r="B65" s="4"/>
       <c r="C65" s="1" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="4"/>
       <c r="B66" s="4"/>
       <c r="C66" s="1" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>81</v>
+        <v>120</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="4"/>
       <c r="B67" s="4"/>
       <c r="C67" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>126</v>
+        <v>121</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="4"/>
+      <c r="B68" s="4"/>
+      <c r="C68" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="4"/>
+      <c r="B69" s="4"/>
+      <c r="C69" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B4:B16"/>
+    <mergeCell ref="B4:B17"/>
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="B18:B48"/>
-    <mergeCell ref="B50:B67"/>
-    <mergeCell ref="A2:A67"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B49:D49"/>
+    <mergeCell ref="B19:B50"/>
+    <mergeCell ref="B52:B69"/>
+    <mergeCell ref="A2:A69"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B51:D51"/>
     <mergeCell ref="B3:D3"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -1906,7 +1942,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6:D6"/>
     </sheetView>
   </sheetViews>
@@ -1919,10 +1955,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>131</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>133</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -1949,20 +1985,20 @@
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1987,10 +2023,10 @@
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -2002,10 +2038,10 @@
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>3</v>
@@ -2050,10 +2086,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -2080,70 +2116,70 @@
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -2168,10 +2204,10 @@
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -2183,10 +2219,10 @@
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>3</v>
@@ -2229,22 +2265,22 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -2271,10 +2307,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -2301,40 +2337,40 @@
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -2370,10 +2406,10 @@
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>3</v>
@@ -2383,10 +2419,10 @@
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -2423,10 +2459,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -2453,10 +2489,10 @@
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2481,10 +2517,10 @@
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -2496,10 +2532,10 @@
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>3</v>
@@ -2545,10 +2581,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -2610,10 +2646,10 @@
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>3</v>
@@ -2623,10 +2659,10 @@
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -2662,10 +2698,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -2727,10 +2763,10 @@
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>3</v>
@@ -2740,10 +2776,10 @@
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>

</xml_diff>